<commit_message>
fitler, non selected and new rules
</commit_message>
<xml_diff>
--- a/Output/PMI_PMP_Charity_Matching_Results_Enhanced.xlsx
+++ b/Output/PMI_PMP_Charity_Matching_Results_Enhanced.xlsx
@@ -12,13 +12,15 @@
     <sheet name="LinkedIn_Analysis" sheetId="3" r:id="rId3"/>
     <sheet name="Enhanced_PMP_Profiles" sheetId="4" r:id="rId4"/>
     <sheet name="Charity_Projects" sheetId="5" r:id="rId5"/>
+    <sheet name="Backup_Candidates" sheetId="6" r:id="rId6"/>
+    <sheet name="Non_Selected_Candidates" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="297">
   <si>
     <t>Charity_Organization</t>
   </si>
@@ -71,90 +73,90 @@
     <t>Overall_PMP_Rating</t>
   </si>
   <si>
+    <t>Drummoyne Community Centre Inc</t>
+  </si>
+  <si>
+    <t>GFG Foundation</t>
+  </si>
+  <si>
+    <t>Sir David Martin Foundation</t>
+  </si>
+  <si>
+    <t>MTC Future Ready</t>
+  </si>
+  <si>
+    <t>Cleaning Accountability Framework (CAF)</t>
+  </si>
+  <si>
     <t>Legacy Club Services</t>
   </si>
   <si>
-    <t>Sir David Martin Foundation</t>
-  </si>
-  <si>
-    <t>MTC Future Ready</t>
-  </si>
-  <si>
     <t>Property Industry Foundation</t>
   </si>
   <si>
-    <t>Cleaning Accountability Framework (CAF)</t>
-  </si>
-  <si>
-    <t>Drummoyne Community Centre Inc</t>
-  </si>
-  <si>
-    <t>GFG Foundation</t>
-  </si>
-  <si>
     <t>Rev. Bill Crews Foundation</t>
   </si>
   <si>
     <t>Total Environment Centre</t>
   </si>
   <si>
+    <t>50th Anniversary of DCC</t>
+  </si>
+  <si>
+    <t>Youth AOD Knowledge Hub</t>
+  </si>
+  <si>
+    <t>Implementation of PMO</t>
+  </si>
+  <si>
+    <t>Website overhaul</t>
+  </si>
+  <si>
     <t>Business ERP</t>
   </si>
   <si>
-    <t>Youth AOD Knowledge Hub</t>
-  </si>
-  <si>
-    <t>Implementation of PMO</t>
+    <t>Building Projects and Working bee Plans</t>
+  </si>
+  <si>
+    <t>To Be Confirmed</t>
   </si>
   <si>
     <t>Events management</t>
   </si>
   <si>
-    <t>Website overhaul</t>
-  </si>
-  <si>
-    <t>50th Anniversary of DCC</t>
-  </si>
-  <si>
-    <t>To Be Confirmed</t>
-  </si>
-  <si>
     <t>Strategic Focus &amp; Capacity Alignment</t>
   </si>
   <si>
-    <t>Building Projects and Working bee Plans</t>
+    <t>Project plan for anniversary. Includes various projects /activities within.</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>A comprehensive national online resource hub that connects young people experiencing alcohol and oth...</t>
+  </si>
+  <si>
+    <t>Guidance/advice on implementation of PMO</t>
+  </si>
+  <si>
+    <t>Our website needs to be overhauled/rebuilt</t>
   </si>
   <si>
     <t xml:space="preserve">implementation of new accounting software </t>
   </si>
   <si>
-    <t>A comprehensive national online resource hub that connects young people experiencing alcohol and oth...</t>
-  </si>
-  <si>
-    <t>Guidance/advice on implementation of PMO</t>
+    <t>We currently organise a range of small to medium building projects for frontline charities but inter...</t>
+  </si>
+  <si>
+    <t>We are yet to finalise the best initiative or project</t>
   </si>
   <si>
     <t>Strategies to promote sustainable fundraising in alignment with our overall strategic plan: Deliver,...</t>
   </si>
   <si>
-    <t>Our website needs to be overhauled/rebuilt</t>
-  </si>
-  <si>
-    <t>Project plan for anniversary. Includes various projects /activities within.</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>We are yet to finalise the best initiative or project</t>
-  </si>
-  <si>
     <t>TEC staff are stretched across too many roles and tasks, often working in the project rather than on...</t>
   </si>
   <si>
-    <t>We currently organise a range of small to medium building projects for frontline charities but inter...</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -170,22 +172,52 @@
     <t>PMP 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Yanika  Okaeva </t>
+  </si>
+  <si>
+    <t>Indra Halim</t>
+  </si>
+  <si>
+    <t>Shannon Blades</t>
+  </si>
+  <si>
+    <t>Doris  Wang</t>
+  </si>
+  <si>
+    <t>Emma  Voss</t>
+  </si>
+  <si>
+    <t>Jauhar Janjua</t>
+  </si>
+  <si>
+    <t>Hadi Ahmadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibrahim  Dani </t>
+  </si>
+  <si>
+    <t>Dhruv Raniga</t>
+  </si>
+  <si>
+    <t>Nadun Dhanushka</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sameh  Megally </t>
   </si>
   <si>
     <t>Nikki Gittins</t>
   </si>
   <si>
-    <t>Emma  Voss</t>
-  </si>
-  <si>
-    <t>Jauhar Janjua</t>
-  </si>
-  <si>
-    <t>Hadi Ahmadi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ibrahim  Dani </t>
+    <t xml:space="preserve">Laetitia Callegari </t>
+  </si>
+  <si>
+    <t>Lindsey Norris</t>
+  </si>
+  <si>
+    <t>Frederick Xavier</t>
+  </si>
+  <si>
+    <t>Ryan Benedek</t>
   </si>
   <si>
     <t>Abby Thakur Satyanarayan</t>
@@ -194,46 +226,43 @@
     <t>Jacqueline Shen</t>
   </si>
   <si>
-    <t>Dhruv Raniga</t>
-  </si>
-  <si>
-    <t>Nadun Dhanushka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yanika  Okaeva </t>
-  </si>
-  <si>
-    <t>Indra Halim</t>
-  </si>
-  <si>
-    <t>Shannon Blades</t>
-  </si>
-  <si>
-    <t>Doris  Wang</t>
-  </si>
-  <si>
-    <t>Frederick Xavier</t>
-  </si>
-  <si>
-    <t>Ryan Benedek</t>
-  </si>
-  <si>
     <t>Julia Wright</t>
   </si>
   <si>
-    <t>Lindsey Norris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laetitia Callegari </t>
-  </si>
-  <si>
     <t>Arvin Arikathota</t>
   </si>
   <si>
+    <t>4 - 8 Years</t>
+  </si>
+  <si>
     <t>More than 8 Years</t>
   </si>
   <si>
-    <t>4 - 8 Years</t>
+    <t xml:space="preserve">Quikky Move </t>
+  </si>
+  <si>
+    <t>Livingstone</t>
+  </si>
+  <si>
+    <t>Sierra Bravo Group</t>
+  </si>
+  <si>
+    <t>AGSM/ Suncorp Bank</t>
+  </si>
+  <si>
+    <t>Woolworths</t>
+  </si>
+  <si>
+    <t>HellermannTyton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney University </t>
+  </si>
+  <si>
+    <t>Clarté</t>
+  </si>
+  <si>
+    <t>AmplifyD</t>
   </si>
   <si>
     <t xml:space="preserve">Sydney Water </t>
@@ -242,13 +271,13 @@
     <t>Atlassian</t>
   </si>
   <si>
-    <t>Woolworths</t>
-  </si>
-  <si>
-    <t>HellermannTyton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sydney University </t>
+    <t xml:space="preserve">PrimeScope </t>
+  </si>
+  <si>
+    <t>Canva</t>
+  </si>
+  <si>
+    <t>ACM</t>
   </si>
   <si>
     <t xml:space="preserve">MUFG Retirement Services </t>
@@ -257,52 +286,52 @@
     <t>Blue Yonder</t>
   </si>
   <si>
-    <t>Clarté</t>
-  </si>
-  <si>
-    <t>AmplifyD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quikky Move </t>
-  </si>
-  <si>
-    <t>Livingstone</t>
-  </si>
-  <si>
-    <t>Sierra Bravo Group</t>
-  </si>
-  <si>
-    <t>AGSM/ Suncorp Bank</t>
-  </si>
-  <si>
-    <t>Canva</t>
-  </si>
-  <si>
-    <t>ACM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimeScope </t>
-  </si>
-  <si>
     <t>Accenture</t>
   </si>
   <si>
+    <t>Project manager</t>
+  </si>
+  <si>
+    <t>Managing Partner, Sales Operations</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBA candidate/ Project Manager/ Senior Business Analyst </t>
+  </si>
+  <si>
+    <t>Stock Loss Manager, Partnerships</t>
+  </si>
+  <si>
+    <t>Project Engineer</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecturer </t>
+  </si>
+  <si>
+    <t>Strategic Design Consultant</t>
+  </si>
+  <si>
+    <t>Delivery Consultant</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cost Manager </t>
   </si>
   <si>
     <t xml:space="preserve">Snr Principle Program Manager [Technical] </t>
   </si>
   <si>
-    <t>Stock Loss Manager, Partnerships</t>
-  </si>
-  <si>
-    <t>Project Engineer</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lecturer </t>
+    <t>Program Director</t>
+  </si>
+  <si>
+    <t>Staff Technical Program Manager</t>
+  </si>
+  <si>
+    <t>Project Controls Specialist</t>
   </si>
   <si>
     <t xml:space="preserve">Senior Project Manager </t>
@@ -311,52 +340,49 @@
     <t>marketing coordinator</t>
   </si>
   <si>
-    <t>Strategic Design Consultant</t>
-  </si>
-  <si>
-    <t>Delivery Consultant</t>
-  </si>
-  <si>
-    <t>Project manager</t>
-  </si>
-  <si>
-    <t>Managing Partner, Sales Operations</t>
-  </si>
-  <si>
-    <t>Consultant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBA candidate/ Project Manager/ Senior Business Analyst </t>
-  </si>
-  <si>
-    <t>Staff Technical Program Manager</t>
-  </si>
-  <si>
-    <t>Project Controls Specialist</t>
-  </si>
-  <si>
     <t xml:space="preserve">Head of Transformation - Smaart Enablement </t>
   </si>
   <si>
-    <t>Program Director</t>
-  </si>
-  <si>
     <t>Delivery Lead</t>
   </si>
   <si>
+    <t>https://www.linkedin.com/in/yanika-okaeva</t>
+  </si>
+  <si>
+    <t>https://linkedin.com/in/indra-halim</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/shannon-blades</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/doris-x-wang</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/emma-voss-07a91341</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/jauhar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/hadiahmadipmp/</t>
+  </si>
+  <si>
+    <t>Linkedin.com/in/ibrahimdani</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dhruvraniga/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nadun-dhanushka/</t>
+  </si>
+  <si>
     <t>https://www.linkedin.com/in/sameh-megally-8aa66a7b?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
   </si>
   <si>
-    <t>www.linkedin.com/in/emma-voss-07a91341</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/jauhar</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/hadiahmadipmp/</t>
-  </si>
-  <si>
-    <t>Linkedin.com/in/ibrahimdani</t>
+    <t>https://www.linkedin.com/in/freddiexavier</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ryan-benedek/</t>
   </si>
   <si>
     <t>www.linkedin.com/in/abhilashasthakur</t>
@@ -365,100 +391,76 @@
     <t>https://www.linkedin.com/in/jacqueline-shen-5b565917a/</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/dhruvraniga/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/nadun-dhanushka/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/yanika-okaeva</t>
-  </si>
-  <si>
-    <t>https://linkedin.com/in/indra-halim</t>
-  </si>
-  <si>
-    <t>www.linkedin.com/in/shannon-blades</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/doris-x-wang</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/freddiexavier</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/ryan-benedek/</t>
-  </si>
-  <si>
     <t>www.linkedin.com/in/juliawright1</t>
   </si>
   <si>
+    <t>Project Management: 5.0, Strategic Planning: 5.0, Volunteering for a Non-profit Organisation: 5.0</t>
+  </si>
+  <si>
+    <t>Project Management: 5.0, Understanding of Agile Principles: 5.0, Plan and Manage Agile Projects: 5.0</t>
+  </si>
+  <si>
+    <t>Project Management: 5.0, Business Change Management: 5.0, Strategic Planning: 4.0</t>
+  </si>
+  <si>
+    <t>Business Analysis: 5.0, Development of User Requirements: 5.0, Project Management: 3.0</t>
+  </si>
+  <si>
     <t>Project Management: 5.0, Strategic Planning: 5.0, Business Change Management: 5.0</t>
   </si>
   <si>
+    <t>Project Management: 5.0, Strategic Planning: 5.0, Business Analysis: 5.0</t>
+  </si>
+  <si>
+    <t>Strategic Planning: 5.0, Business Analysis: 5.0, Development of User Requirements: 5.0</t>
+  </si>
+  <si>
     <t>Project Management: 5.0, Business Change Management: 5.0, Business Analysis: 5.0</t>
   </si>
   <si>
-    <t>Project Management: 5.0, Strategic Planning: 5.0, Business Analysis: 5.0</t>
+    <t>Project Management: 5.0, Business Analysis: 5.0, Business Change Management: 4.0</t>
+  </si>
+  <si>
+    <t>Project Management: 5.0, Business Analysis: 5.0, Understanding of Agile Principles: 5.0</t>
+  </si>
+  <si>
+    <t>Project Management: 5.0, Portfolio Management: 5.0, Understanding of Agile Principles: 5.0</t>
+  </si>
+  <si>
+    <t>Project Management: 4.0, Business Change Management: 4.0, Business Analysis: 4.0</t>
   </si>
   <si>
     <t>Events Planning and Management: 5.0, Project Management: 4.0, Strategic Planning: 4.0</t>
   </si>
   <si>
-    <t>Strategic Planning: 5.0, Business Analysis: 5.0, Development of User Requirements: 5.0</t>
-  </si>
-  <si>
-    <t>Project Management: 5.0, Understanding of Agile Principles: 5.0, Plan and Manage Agile Projects: 5.0</t>
-  </si>
-  <si>
-    <t>Project Management: 5.0, Strategic Planning: 5.0, Volunteering for a Non-profit Organisation: 5.0</t>
-  </si>
-  <si>
-    <t>Project Management: 5.0, Business Change Management: 5.0, Strategic Planning: 4.0</t>
-  </si>
-  <si>
-    <t>Business Analysis: 5.0, Development of User Requirements: 5.0, Project Management: 3.0</t>
-  </si>
-  <si>
-    <t>Project Management: 5.0, Portfolio Management: 5.0, Understanding of Agile Principles: 5.0</t>
-  </si>
-  <si>
-    <t>Project Management: 4.0, Business Change Management: 4.0, Business Analysis: 4.0</t>
-  </si>
-  <si>
     <t>Project Management: 5.0, Strategic Planning: 5.0, Portfolio Management: 5.0</t>
   </si>
   <si>
-    <t>Project Management: 5.0, Business Analysis: 5.0, Understanding of Agile Principles: 5.0</t>
-  </si>
-  <si>
-    <t>Project Management: 5.0, Business Analysis: 5.0, Business Change Management: 4.0</t>
+    <t>Events Planning and Management: 10, Project Management: 4, Volunteering for a Non-profit Organisation: 4</t>
+  </si>
+  <si>
+    <t>Volunteering for a Non-profit Organisation: 2</t>
+  </si>
+  <si>
+    <t>Strategic Planning: 10, Volunteering for a Non-profit Organisation: 6, Project Management: 4</t>
+  </si>
+  <si>
+    <t>Business Change Management: 9</t>
+  </si>
+  <si>
+    <t>Strategic Planning: 2, Development of User Requirements: 2</t>
   </si>
   <si>
     <t>Business Analysis: 7, Strategic Planning: 4, Business Change Management: 4</t>
   </si>
   <si>
-    <t>Strategic Planning: 10, Volunteering for a Non-profit Organisation: 6, Project Management: 4</t>
-  </si>
-  <si>
-    <t>Business Change Management: 9</t>
+    <t>Business Analysis: 4, Volunteering for a Non-profit Organisation: 4, Strategic Planning: 2</t>
   </si>
   <si>
     <t>Events Planning and Management: 10, Strategic Planning: 8, Business Analysis: 2</t>
   </si>
   <si>
-    <t>Strategic Planning: 2, Development of User Requirements: 2</t>
-  </si>
-  <si>
-    <t>Events Planning and Management: 10, Project Management: 4, Volunteering for a Non-profit Organisation: 4</t>
-  </si>
-  <si>
-    <t>Volunteering for a Non-profit Organisation: 2</t>
-  </si>
-  <si>
     <t>Strategic Planning: 10, Events Planning and Management: 4, Project Management: 2</t>
-  </si>
-  <si>
-    <t>Business Analysis: 4, Volunteering for a Non-profit Organisation: 4, Strategic Planning: 2</t>
   </si>
   <si>
     <t>Organization</t>
@@ -486,142 +488,142 @@
 Building on our Phase 1 work with the Alcohol and Drug Foundation focused on identifying youth-specific AOD services in Australia, we aim to transform how young Australians access AOD support by creating a centralised, user-friendly platform that guides them to appropriate local services and resources.</t>
   </si>
   <si>
+    <t xml:space="preserve">We currently organise a range of small to medium building projects for frontline charities but internally we do not have any expertise on project building management. Having a template or system to guide us would be great. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Strategies to promote sustainable fundraising in alignment with our overall strategic plan: Deliver, Amplify, Transform. </t>
   </si>
   <si>
     <t>TEC staff are stretched across too many roles and tasks, often working in the project rather than on it. Limited leadership and management capacity mean that opportunities are sometimes pursued without clear prioritisation, leading to overstretch, inefficiency, and reduced impact.</t>
   </si>
   <si>
-    <t xml:space="preserve">We currently organise a range of small to medium building projects for frontline charities but internally we do not have any expertise on project building management. Having a template or system to guide us would be great. </t>
+    <t>Project Management, Volunteering for a Non-profit Organisation, Events Planning and Management</t>
+  </si>
+  <si>
+    <t>Project Management, Strategic Planning, Volunteering for a Non-profit Organisation, Systems Integration (Business and Technical)</t>
+  </si>
+  <si>
+    <t>Business Change Management</t>
   </si>
   <si>
     <t>Strategic Planning, Business Change Management, Business Analysis, Technology Change Management, Planning &amp; Management of the Implementation of New Software Solutions</t>
   </si>
   <si>
-    <t>Project Management, Strategic Planning, Volunteering for a Non-profit Organisation, Systems Integration (Business and Technical)</t>
-  </si>
-  <si>
-    <t>Business Change Management</t>
+    <t>Business Analysis, Volunteering for a Non-profit Organisation</t>
   </si>
   <si>
     <t>Strategic Planning, Events Planning and Management</t>
   </si>
   <si>
-    <t>Project Management, Volunteering for a Non-profit Organisation, Events Planning and Management</t>
-  </si>
-  <si>
-    <t>Business Analysis, Volunteering for a Non-profit Organisation</t>
+    <t>Yanika  Okaeva  | Indra Halim</t>
+  </si>
+  <si>
+    <t>Shannon Blades | Doris  Wang</t>
+  </si>
+  <si>
+    <t>Emma  Voss | Jauhar Janjua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hadi Ahmadi | Ibrahim  Dani </t>
+  </si>
+  <si>
+    <t>Dhruv Raniga | Nadun Dhanushka</t>
   </si>
   <si>
     <t>Sameh  Megally  | Nikki Gittins</t>
   </si>
   <si>
-    <t>Emma  Voss | Jauhar Janjua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hadi Ahmadi | Ibrahim  Dani </t>
+    <t>Laetitia Callegari  | Lindsey Norris</t>
+  </si>
+  <si>
+    <t>Frederick Xavier | Ryan Benedek</t>
   </si>
   <si>
     <t>Abby Thakur Satyanarayan | Jacqueline Shen</t>
   </si>
   <si>
-    <t>Dhruv Raniga | Nadun Dhanushka</t>
-  </si>
-  <si>
-    <t>Yanika  Okaeva  | Indra Halim</t>
-  </si>
-  <si>
-    <t>Shannon Blades | Doris  Wang</t>
-  </si>
-  <si>
-    <t>Frederick Xavier | Ryan Benedek</t>
-  </si>
-  <si>
-    <t>Julia Wright | Lindsey Norris</t>
-  </si>
-  <si>
-    <t>Laetitia Callegari  | Arvin Arikathota</t>
+    <t>Julia Wright | Arvin Arikathota</t>
+  </si>
+  <si>
+    <t>86.32 | 86.32</t>
+  </si>
+  <si>
+    <t>81.82 | 80.0</t>
+  </si>
+  <si>
+    <t>92.96 | 91.11</t>
+  </si>
+  <si>
+    <t>89.66 | 87.59</t>
+  </si>
+  <si>
+    <t>87.5 | 84.17</t>
   </si>
   <si>
     <t>93.02 | 81.4</t>
   </si>
   <si>
-    <t>92.96 | 91.11</t>
-  </si>
-  <si>
-    <t>89.66 | 87.59</t>
+    <t>74.12 | 74.12</t>
+  </si>
+  <si>
+    <t>79.09 | 75.45</t>
   </si>
   <si>
     <t>89.05 | 80.0</t>
   </si>
   <si>
-    <t>87.5 | 84.17</t>
-  </si>
-  <si>
-    <t>86.32 | 86.32</t>
-  </si>
-  <si>
-    <t>81.82 | 80.0</t>
-  </si>
-  <si>
-    <t>79.09 | 75.45</t>
-  </si>
-  <si>
-    <t>78.26 | 77.39</t>
-  </si>
-  <si>
-    <t>74.12 | 72.94</t>
+    <t>78.26 | 75.65</t>
+  </si>
+  <si>
+    <t>10 | 10</t>
+  </si>
+  <si>
+    <t>8 | 10</t>
+  </si>
+  <si>
+    <t>8 | 8</t>
+  </si>
+  <si>
+    <t>10 | 8</t>
   </si>
   <si>
     <t>10 | 0</t>
   </si>
   <si>
-    <t>8 | 8</t>
-  </si>
-  <si>
-    <t>10 | 8</t>
-  </si>
-  <si>
-    <t>8 | 10</t>
-  </si>
-  <si>
-    <t>10 | 10</t>
+    <t>0 | 0</t>
   </si>
   <si>
     <t>8 | 0</t>
   </si>
   <si>
-    <t>0 | 0</t>
+    <t xml:space="preserve">PMP 1 (Yanika  Okaeva ) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Volunteering for a Non-profit Organisation (PMP: 5.0/5, Required: 4). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Indra Halim) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Volunteering for a Non-profit Organisation (PMP: 5.0/5, Required: 4). High-quality LinkedIn profile. Complete professional profile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMP 1 (Shannon Blades) selected because: Strong skills in Volunteering for a Non-profit Organisation (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Doris  Wang) selected because: Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMP 1 (Emma  Voss) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Strategic Planning (PMP: 5.0/5, Required: 10). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Jauhar Janjua) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Strategic Planning (PMP: 5.0/5, Required: 10). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMP 1 (Hadi Ahmadi) selected because: Strong skills in Business Change Management (PMP: 5.0/5, Required: 9). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Ibrahim  Dani ) selected because: Strong skills in Business Change Management (PMP: 5.0/5, Required: 9). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMP 1 (Dhruv Raniga) selected because: Strong skills in Strategic Planning (PMP: 5.0/5, Required: 2); Development of User Requirements (PMP: 5.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Nadun Dhanushka) selected because: Strong skills in Strategic Planning (PMP: 4.0/5, Required: 2); Development of User Requirements (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
   </si>
   <si>
     <t xml:space="preserve">PMP 1 (Sameh  Megally ) selected because: Strong skills in Strategic Planning (PMP: 5.0/5, Required: 4); Business Change Management (PMP: 5.0/5, Required: 4). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Nikki Gittins) selected because: Strong skills in Business Change Management (PMP: 5.0/5, Required: 4); Business Analysis (PMP: 5.0/5, Required: 7). Extensive experience (8+ years). Complete professional profile. </t>
   </si>
   <si>
-    <t xml:space="preserve">PMP 1 (Emma  Voss) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Strategic Planning (PMP: 5.0/5, Required: 10). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Jauhar Janjua) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Strategic Planning (PMP: 5.0/5, Required: 10). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMP 1 (Hadi Ahmadi) selected because: Strong skills in Business Change Management (PMP: 5.0/5, Required: 9). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Ibrahim  Dani ) selected because: Strong skills in Business Change Management (PMP: 5.0/5, Required: 9). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
+    <t xml:space="preserve">PMP 1 (Laetitia Callegari ) selected because: Strong skills in Business Analysis (PMP: 5.0/5, Required: 4); Technology Change Management (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). Complete professional profile.  | PMP 2 (Lindsey Norris) selected because: Strong skills in Strategic Planning (PMP: 4.0/5, Required: 2); Business Analysis (PMP: 5.0/5, Required: 4). Extensive experience (8+ years). Complete professional profile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMP 1 (Frederick Xavier) selected because: Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Ryan Benedek) selected because: Strong skills in Volunteering for a Non-profit Organisation (PMP: 4.0/5, Required: 2). High-quality LinkedIn profile. Complete professional profile. </t>
   </si>
   <si>
     <t xml:space="preserve">PMP 1 (Abby Thakur Satyanarayan) selected because: Strong skills in Strategic Planning (PMP: 5.0/5, Required: 8); Business Analysis (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Jacqueline Shen) selected because: Strong skills in Strategic Planning (PMP: 4.0/5, Required: 8); Events Planning and Management (PMP: 5.0/5, Required: 10). High-quality LinkedIn profile. Complete professional profile. </t>
   </si>
   <si>
-    <t xml:space="preserve">PMP 1 (Dhruv Raniga) selected because: Strong skills in Strategic Planning (PMP: 5.0/5, Required: 2); Development of User Requirements (PMP: 5.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Nadun Dhanushka) selected because: Strong skills in Strategic Planning (PMP: 4.0/5, Required: 2); Development of User Requirements (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMP 1 (Yanika  Okaeva ) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Volunteering for a Non-profit Organisation (PMP: 5.0/5, Required: 4). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Indra Halim) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 4); Volunteering for a Non-profit Organisation (PMP: 5.0/5, Required: 4). High-quality LinkedIn profile. Complete professional profile. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMP 1 (Shannon Blades) selected because: Strong skills in Volunteering for a Non-profit Organisation (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Doris  Wang) selected because: Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMP 1 (Frederick Xavier) selected because: Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Ryan Benedek) selected because: Strong skills in Volunteering for a Non-profit Organisation (PMP: 4.0/5, Required: 2). High-quality LinkedIn profile. Complete professional profile. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMP 1 (Julia Wright) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 2); Strategic Planning (PMP: 5.0/5, Required: 10). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Lindsey Norris) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 2); Strategic Planning (PMP: 4.0/5, Required: 10). Extensive experience (8+ years). Complete professional profile. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMP 1 (Laetitia Callegari ) selected because: Strong skills in Business Analysis (PMP: 5.0/5, Required: 4); Technology Change Management (PMP: 4.0/5, Required: 2). Extensive experience (8+ years). Complete professional profile.  | PMP 2 (Arvin Arikathota) selected because: Strong skills in Strategic Planning (PMP: 4.0/5, Required: 2); Business Analysis (PMP: 4.0/5, Required: 4). Extensive experience (8+ years). Complete professional profile. </t>
+    <t xml:space="preserve">PMP 1 (Julia Wright) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 2); Strategic Planning (PMP: 5.0/5, Required: 10). Extensive experience (8+ years). High-quality LinkedIn profile. Complete professional profile.  | PMP 2 (Arvin Arikathota) selected because: Strong skills in Project Management (PMP: 5.0/5, Required: 2); Strategic Planning (PMP: 4.0/5, Required: 10). Extensive experience (8+ years). Complete professional profile. </t>
   </si>
   <si>
     <t>Name</t>
@@ -853,6 +855,63 @@
   </si>
   <si>
     <t>Complexity</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Best_Match</t>
+  </si>
+  <si>
+    <t>Best_Score</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>neha_purohit08@outlook.com</t>
+  </si>
+  <si>
+    <t>reddysuresh27@gmail.com</t>
+  </si>
+  <si>
+    <t>reddyshailu24@gmail.com</t>
+  </si>
+  <si>
+    <t>shreya.shah@student.unsw.edu.au</t>
+  </si>
+  <si>
+    <t>pharris3@optusnet.com.au</t>
+  </si>
+  <si>
+    <t>carolmelo.pm@gmail.com</t>
+  </si>
+  <si>
+    <t>ivonne.portoc@gmail.com</t>
+  </si>
+  <si>
+    <t>RDA.JOHN@gmail.com</t>
+  </si>
+  <si>
+    <t>achintyah619@gmail.com</t>
+  </si>
+  <si>
+    <t>dsookharee@northrop.com.au</t>
+  </si>
+  <si>
+    <t>Qualified - awaiting assignment</t>
+  </si>
+  <si>
+    <t>Backup Candidate</t>
+  </si>
+  <si>
+    <t>mirna.alemadi@gmail.com</t>
+  </si>
+  <si>
+    <t>aishwarya.rajendran2012@gmail.com</t>
+  </si>
+  <si>
+    <t>Non-selected</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1383,7 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -1348,10 +1407,10 @@
         <v>10</v>
       </c>
       <c r="M2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N2">
-        <v>93.02</v>
+        <v>86.31999999999999</v>
       </c>
       <c r="O2" t="s">
         <v>124</v>
@@ -1360,7 +1419,7 @@
         <v>138</v>
       </c>
       <c r="Q2">
-        <v>5.04</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1377,7 +1436,7 @@
         <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>49</v>
@@ -1394,14 +1453,17 @@
       <c r="J3" t="s">
         <v>90</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="L3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N3">
-        <v>81.40000000000001</v>
+        <v>86.31999999999999</v>
       </c>
       <c r="O3" t="s">
         <v>125</v>
@@ -1410,24 +1472,21 @@
         <v>138</v>
       </c>
       <c r="Q3">
-        <v>4.94</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
       <c r="C4" t="s">
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
         <v>48</v>
@@ -1436,7 +1495,7 @@
         <v>52</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
         <v>74</v>
@@ -1445,42 +1504,39 @@
         <v>91</v>
       </c>
       <c r="K4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L4">
         <v>8</v>
       </c>
       <c r="M4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N4">
-        <v>92.95999999999999</v>
+        <v>81.81999999999999</v>
       </c>
       <c r="O4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="P4" t="s">
         <v>139</v>
       </c>
       <c r="Q4">
-        <v>6.25</v>
+        <v>4.68</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
       <c r="C5" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
@@ -1489,7 +1545,7 @@
         <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
         <v>75</v>
@@ -1497,26 +1553,26 @@
       <c r="J5" t="s">
         <v>92</v>
       </c>
-      <c r="K5" t="s">
-        <v>110</v>
+      <c r="K5" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="L5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N5">
-        <v>91.11</v>
+        <v>80</v>
       </c>
       <c r="O5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P5" t="s">
         <v>139</v>
       </c>
       <c r="Q5">
-        <v>5.99</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1524,16 +1580,16 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
         <v>48</v>
@@ -1542,34 +1598,34 @@
         <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>111</v>
+      <c r="K6" t="s">
+        <v>112</v>
       </c>
       <c r="L6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N6">
-        <v>89.66</v>
+        <v>92.95999999999999</v>
       </c>
       <c r="O6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="P6" t="s">
         <v>140</v>
       </c>
       <c r="Q6">
-        <v>5.81</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1577,16 +1633,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>49</v>
@@ -1595,16 +1651,16 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J7" t="s">
         <v>94</v>
       </c>
       <c r="K7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L7">
         <v>8</v>
@@ -1613,16 +1669,16 @@
         <v>10</v>
       </c>
       <c r="N7">
-        <v>87.59</v>
+        <v>91.11</v>
       </c>
       <c r="O7" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="P7" t="s">
         <v>140</v>
       </c>
       <c r="Q7">
-        <v>5.07</v>
+        <v>5.99</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1630,16 +1686,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
         <v>48</v>
@@ -1648,34 +1704,34 @@
         <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s">
         <v>95</v>
       </c>
-      <c r="K8" t="s">
-        <v>113</v>
+      <c r="K8" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="L8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N8">
-        <v>89.05</v>
+        <v>89.66</v>
       </c>
       <c r="O8" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="P8" t="s">
         <v>141</v>
       </c>
       <c r="Q8">
-        <v>5.56</v>
+        <v>5.81</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1683,16 +1739,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
@@ -1709,26 +1765,26 @@
       <c r="J9" t="s">
         <v>96</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>114</v>
+      <c r="K9" t="s">
+        <v>115</v>
       </c>
       <c r="L9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N9">
-        <v>80</v>
+        <v>87.59</v>
       </c>
       <c r="O9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="P9" t="s">
         <v>141</v>
       </c>
       <c r="Q9">
-        <v>4.37</v>
+        <v>5.07</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1736,7 +1792,7 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1754,7 +1810,7 @@
         <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I10" t="s">
         <v>79</v>
@@ -1763,7 +1819,7 @@
         <v>97</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L10">
         <v>10</v>
@@ -1775,7 +1831,7 @@
         <v>87.5</v>
       </c>
       <c r="O10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="P10" t="s">
         <v>142</v>
@@ -1789,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>39</v>
@@ -1807,7 +1863,7 @@
         <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
         <v>80</v>
@@ -1816,7 +1872,7 @@
         <v>98</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L11">
         <v>10</v>
@@ -1828,7 +1884,7 @@
         <v>84.17</v>
       </c>
       <c r="O11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="P11" t="s">
         <v>142</v>
@@ -1842,7 +1898,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
@@ -1851,7 +1907,7 @@
         <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
         <v>48</v>
@@ -1869,25 +1925,25 @@
         <v>99</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L12">
         <v>10</v>
       </c>
       <c r="M12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N12">
-        <v>86.31999999999999</v>
+        <v>93.02</v>
       </c>
       <c r="O12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P12" t="s">
         <v>143</v>
       </c>
       <c r="Q12">
-        <v>4.53</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1895,7 +1951,7 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
@@ -1904,7 +1960,7 @@
         <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
         <v>49</v>
@@ -1921,32 +1977,32 @@
       <c r="J13" t="s">
         <v>100</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="L13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N13">
-        <v>86.31999999999999</v>
+        <v>81.40000000000001</v>
       </c>
       <c r="O13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="P13" t="s">
         <v>143</v>
       </c>
       <c r="Q13">
-        <v>5.68</v>
+        <v>4.94</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>23</v>
       </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
       <c r="C14" t="s">
         <v>41</v>
       </c>
@@ -1963,7 +2019,7 @@
         <v>62</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
         <v>83</v>
@@ -1971,32 +2027,32 @@
       <c r="J14" t="s">
         <v>101</v>
       </c>
-      <c r="K14" t="s">
-        <v>119</v>
-      </c>
       <c r="L14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N14">
-        <v>81.81999999999999</v>
+        <v>74.12</v>
       </c>
       <c r="O14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="P14" t="s">
         <v>144</v>
       </c>
       <c r="Q14">
-        <v>4.68</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>23</v>
       </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
       <c r="C15" t="s">
         <v>41</v>
       </c>
@@ -2013,34 +2069,31 @@
         <v>63</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="J15" t="s">
-        <v>102</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="L15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N15">
-        <v>80</v>
+        <v>74.12</v>
       </c>
       <c r="O15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="P15" t="s">
         <v>144</v>
       </c>
       <c r="Q15">
-        <v>3.83</v>
+        <v>4.71</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2066,16 +2119,16 @@
         <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L16">
         <v>10</v>
@@ -2087,10 +2140,10 @@
         <v>79.09</v>
       </c>
       <c r="O16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="P16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="Q16">
         <v>4.73</v>
@@ -2119,16 +2172,16 @@
         <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L17">
         <v>10</v>
@@ -2140,10 +2193,10 @@
         <v>75.45</v>
       </c>
       <c r="O17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="Q17">
         <v>4.5</v>
@@ -2151,7 +2204,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -2163,7 +2216,7 @@
         <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
         <v>48</v>
@@ -2172,39 +2225,39 @@
         <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="J18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L18">
         <v>8</v>
       </c>
       <c r="M18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N18">
-        <v>78.26000000000001</v>
+        <v>89.05</v>
       </c>
       <c r="O18" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="P18" t="s">
         <v>145</v>
       </c>
       <c r="Q18">
-        <v>4.84</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
@@ -2216,7 +2269,7 @@
         <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
         <v>49</v>
@@ -2228,19 +2281,22 @@
         <v>70</v>
       </c>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="J19" t="s">
-        <v>93</v>
+        <v>105</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N19">
-        <v>77.39</v>
+        <v>80</v>
       </c>
       <c r="O19" t="s">
         <v>136</v>
@@ -2249,12 +2305,12 @@
         <v>145</v>
       </c>
       <c r="Q19">
-        <v>4.71</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
@@ -2263,7 +2319,7 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>47</v>
@@ -2275,22 +2331,25 @@
         <v>68</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J20" t="s">
         <v>106</v>
       </c>
+      <c r="K20" t="s">
+        <v>123</v>
+      </c>
       <c r="L20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N20">
-        <v>74.12</v>
+        <v>78.26000000000001</v>
       </c>
       <c r="O20" t="s">
         <v>137</v>
@@ -2299,12 +2358,12 @@
         <v>146</v>
       </c>
       <c r="Q20">
-        <v>4.32</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -2313,7 +2372,7 @@
         <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -2325,7 +2384,7 @@
         <v>69</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
         <v>88</v>
@@ -2340,10 +2399,10 @@
         <v>8</v>
       </c>
       <c r="N21">
-        <v>72.94</v>
+        <v>75.65000000000001</v>
       </c>
       <c r="O21" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="P21" t="s">
         <v>146</v>
@@ -2355,15 +2414,15 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K6" r:id="rId2"/>
-    <hyperlink ref="K9" r:id="rId3"/>
-    <hyperlink ref="K10" r:id="rId4"/>
-    <hyperlink ref="K11" r:id="rId5"/>
-    <hyperlink ref="K12" r:id="rId6"/>
-    <hyperlink ref="K13" r:id="rId7"/>
-    <hyperlink ref="K15" r:id="rId8"/>
-    <hyperlink ref="K16" r:id="rId9"/>
-    <hyperlink ref="K17" r:id="rId10"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K5" r:id="rId3"/>
+    <hyperlink ref="K8" r:id="rId4"/>
+    <hyperlink ref="K10" r:id="rId5"/>
+    <hyperlink ref="K11" r:id="rId6"/>
+    <hyperlink ref="K12" r:id="rId7"/>
+    <hyperlink ref="K16" r:id="rId8"/>
+    <hyperlink ref="K17" r:id="rId9"/>
+    <hyperlink ref="K19" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2443,14 +2502,8 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>165</v>
@@ -2470,13 +2523,13 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
         <v>166</v>
@@ -2496,13 +2549,13 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
         <v>167</v>
@@ -2522,7 +2575,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
@@ -2534,7 +2587,7 @@
         <v>178</v>
       </c>
       <c r="G6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H6" t="s">
         <v>195</v>
@@ -2545,13 +2598,13 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
         <v>169</v>
@@ -2570,8 +2623,14 @@
       <c r="A8" t="s">
         <v>23</v>
       </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>155</v>
+      </c>
+      <c r="D8" t="s">
+        <v>162</v>
       </c>
       <c r="E8" t="s">
         <v>170</v>
@@ -2580,7 +2639,7 @@
         <v>180</v>
       </c>
       <c r="G8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H8" t="s">
         <v>197</v>
@@ -2603,7 +2662,7 @@
         <v>181</v>
       </c>
       <c r="G9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="H9" t="s">
         <v>198</v>
@@ -2611,7 +2670,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -2620,7 +2679,7 @@
         <v>156</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E10" t="s">
         <v>172</v>
@@ -2629,7 +2688,7 @@
         <v>182</v>
       </c>
       <c r="G10" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H10" t="s">
         <v>199</v>
@@ -2637,7 +2696,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -2751,10 +2810,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -2763,10 +2822,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G4">
         <v>3.83</v>
@@ -2774,10 +2833,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -2786,10 +2845,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G5">
         <v>4.53</v>
@@ -2797,10 +2856,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -2809,10 +2868,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G6">
         <v>5.99</v>
@@ -2820,10 +2879,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -2832,10 +2891,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G7">
         <v>5.07</v>
@@ -2863,7 +2922,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2872,10 +2931,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G9">
         <v>4.32</v>
@@ -2886,7 +2945,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -2955,7 +3014,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -2964,10 +3023,10 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13">
         <v>4.73</v>
@@ -2990,7 +3049,7 @@
         <v>228</v>
       </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G14">
         <v>3.84</v>
@@ -2998,10 +3057,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C15">
         <v>8</v>
@@ -3010,10 +3069,10 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G15">
         <v>5.56</v>
@@ -3021,10 +3080,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -3033,10 +3092,10 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G16">
         <v>5.68</v>
@@ -3044,10 +3103,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -3056,10 +3115,10 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G17">
         <v>4.68</v>
@@ -3082,7 +3141,7 @@
         <v>230</v>
       </c>
       <c r="F18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G18">
         <v>3.1</v>
@@ -3093,7 +3152,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -3102,10 +3161,10 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G19">
         <v>4.5</v>
@@ -3113,10 +3172,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C20">
         <v>10</v>
@@ -3125,10 +3184,10 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="G20">
         <v>4.37</v>
@@ -3136,7 +3195,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -3145,10 +3204,10 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="G21">
         <v>4.94</v>
@@ -3251,7 +3310,7 @@
         <v>235</v>
       </c>
       <c r="F26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G26">
         <v>3.94</v>
@@ -3259,10 +3318,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -3271,10 +3330,10 @@
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="G27">
         <v>5.04</v>
@@ -3305,7 +3364,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
         <v>123</v>
@@ -3317,10 +3376,10 @@
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G29">
         <v>4.84</v>
@@ -3328,10 +3387,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C30">
         <v>8</v>
@@ -3340,10 +3399,10 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G30">
         <v>6.25</v>
@@ -3351,7 +3410,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -3360,10 +3419,10 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G31">
         <v>4.71</v>
@@ -3371,10 +3430,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -3383,10 +3442,10 @@
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G32">
         <v>5.81</v>
@@ -3397,7 +3456,7 @@
         <v>58</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -3483,7 +3542,7 @@
         <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -3526,10 +3585,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3549,10 +3608,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -3572,10 +3631,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -3595,10 +3654,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -3621,7 +3680,7 @@
         <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3641,10 +3700,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3667,7 +3726,7 @@
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -3690,7 +3749,7 @@
         <v>209</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -3736,7 +3795,7 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -3759,7 +3818,7 @@
         <v>211</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14">
         <v>8</v>
@@ -3779,10 +3838,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15">
         <v>8</v>
@@ -3802,10 +3861,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -3825,10 +3884,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -3851,7 +3910,7 @@
         <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18">
         <v>8</v>
@@ -3874,7 +3933,7 @@
         <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19">
         <v>10</v>
@@ -3894,10 +3953,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -3917,10 +3976,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -3943,7 +4002,7 @@
         <v>213</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3989,7 +4048,7 @@
         <v>215</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4012,7 +4071,7 @@
         <v>216</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -4035,7 +4094,7 @@
         <v>217</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -4055,10 +4114,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -4101,10 +4160,10 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29">
         <v>8</v>
@@ -4124,10 +4183,10 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30">
         <v>8</v>
@@ -4147,10 +4206,10 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -4170,10 +4229,10 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32">
         <v>10</v>
@@ -4196,7 +4255,7 @@
         <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33">
         <v>10</v>
@@ -4253,10 +4312,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -4270,7 +4329,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
@@ -4284,7 +4343,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -4301,7 +4360,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -4321,7 +4380,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
@@ -4335,10 +4394,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
@@ -4352,10 +4411,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
@@ -4386,10 +4445,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -4406,13 +4465,464 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>82.06999999999999</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>66.31999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>73.68000000000001</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>68.18000000000001</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>68.52</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>78.62</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>70.91</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>71.84999999999999</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>76.31999999999999</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>58.42</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>38.18</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>40.91</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>